<commit_message>
Adding data and code
</commit_message>
<xml_diff>
--- a/src/main/java/pageObjectModel/automation/data/Login.xlsx
+++ b/src/main/java/pageObjectModel/automation/data/Login.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Y</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>verificationMessage</t>
-  </si>
-  <si>
-    <t>Welcome123 to your account. Here you can manage all of your personal information and orders.</t>
   </si>
   <si>
     <t>Welcome to your account. Here you can manage all of your personal information and orders.</t>
@@ -151,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +158,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -177,10 +180,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +489,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F2" sqref="F2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -511,10 +515,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -542,14 +546,14 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>2017</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -558,10 +562,10 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s">
         <v>0</v>
@@ -577,23 +581,23 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
-        <v>2019</v>
+      <c r="D3" s="2">
+        <v>2016</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
         <v>13</v>
@@ -612,26 +616,26 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4">
-        <v>2016</v>
+      <c r="D4" s="2">
+        <v>2015</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K4" t="s">
         <v>0</v>
@@ -647,29 +651,29 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
-        <v>2020</v>
+      <c r="D5" s="2">
+        <v>2014</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
         <v>13</v>
       </c>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding code to framework
</commit_message>
<xml_diff>
--- a/src/main/java/pageObjectModel/automation/data/Login.xlsx
+++ b/src/main/java/pageObjectModel/automation/data/Login.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Registor" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>Welcome to your account. Here you can manage all of your personal information and orders.</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>customerfirstName</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>addresslll</t>
+  </si>
+  <si>
+    <t>Welcome123 to your account. Here you can manage all of your personal information and orders.</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -515,10 +515,10 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -550,10 +550,10 @@
         <v>2017</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
         <v>5</v>
@@ -562,7 +562,7 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
@@ -585,19 +585,19 @@
         <v>2016</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
         <v>13</v>
@@ -620,19 +620,19 @@
         <v>2015</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
@@ -655,25 +655,25 @@
         <v>2014</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
         <v>32</v>
       </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
       <c r="K5" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>